<commit_message>
flag for test mode recipients
</commit_message>
<xml_diff>
--- a/attachments/fmt/tabellen/tab.xlsx
+++ b/attachments/fmt/tabellen/tab.xlsx
@@ -5,26 +5,26 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSC\Documents\ZEW\projekte\FMT Deutschland\FMT-10-22\Ergebnisse\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MSC\Documents\ZEW\projekte\FMT Deutschland\FMT-11-22\Ergebnisse\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8952"/>
   </bookViews>
   <sheets>
-    <sheet name="tab-2022-10" sheetId="1" r:id="rId1"/>
+    <sheet name="tab-2022-11" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="175">
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>ZEW - Finanzmarkttest Oktober 2022: Belegung der Antwortkategorien</t>
+    <t>ZEW - Finanzmarkttest November 2022: Belegung der Antwortkategorien</t>
   </si>
   <si>
     <t>Konjunktur (Situation)</t>
@@ -45,436 +45,499 @@
     <t>Euroraum</t>
   </si>
   <si>
-    <t>(- 1.3)</t>
+    <t>(+ 0.9)</t>
+  </si>
+  <si>
+    <t>(+ 3.7)</t>
+  </si>
+  <si>
+    <t>(- 4.6)</t>
+  </si>
+  <si>
+    <t>(+ 5.5)</t>
+  </si>
+  <si>
+    <t>Deutschland</t>
+  </si>
+  <si>
+    <t>(+ 0.4)</t>
+  </si>
+  <si>
+    <t>(+ 6.9)</t>
+  </si>
+  <si>
+    <t>(- 7.3)</t>
+  </si>
+  <si>
+    <t>(+ 7.7)</t>
+  </si>
+  <si>
+    <t>USA</t>
+  </si>
+  <si>
+    <t>(- 1.5)</t>
+  </si>
+  <si>
+    <t>(+ 8.9)</t>
+  </si>
+  <si>
+    <t>(- 7.4)</t>
+  </si>
+  <si>
+    <t>(+ 5.9)</t>
+  </si>
+  <si>
+    <t>China</t>
+  </si>
+  <si>
+    <t>(+ 1.2)</t>
+  </si>
+  <si>
+    <t>(+ 0.6)</t>
+  </si>
+  <si>
+    <t>(- 1.8)</t>
+  </si>
+  <si>
+    <t>(+ 3.0)</t>
+  </si>
+  <si>
+    <t>Konjunktur (Erwartungen)</t>
+  </si>
+  <si>
+    <t>verbessern</t>
+  </si>
+  <si>
+    <t>nicht verändern</t>
+  </si>
+  <si>
+    <t>verschlechtern</t>
+  </si>
+  <si>
+    <t>(+ 5.1)</t>
+  </si>
+  <si>
+    <t>(+10.8)</t>
+  </si>
+  <si>
+    <t>(-15.9)</t>
+  </si>
+  <si>
+    <t>(+21.0)</t>
+  </si>
+  <si>
+    <t>(+11.5)</t>
+  </si>
+  <si>
+    <t>(-17.0)</t>
+  </si>
+  <si>
+    <t>(+22.5)</t>
+  </si>
+  <si>
+    <t>(+ 4.0)</t>
+  </si>
+  <si>
+    <t>(+ 2.1)</t>
+  </si>
+  <si>
+    <t>(- 6.1)</t>
+  </si>
+  <si>
+    <t>(+10.1)</t>
+  </si>
+  <si>
+    <t>(+ 9.0)</t>
+  </si>
+  <si>
+    <t>(- 2.4)</t>
+  </si>
+  <si>
+    <t>(- 6.6)</t>
+  </si>
+  <si>
+    <t>(+15.6)</t>
+  </si>
+  <si>
+    <t>Inflationsrate</t>
+  </si>
+  <si>
+    <t>erhöhen</t>
+  </si>
+  <si>
+    <t>reduzieren</t>
+  </si>
+  <si>
+    <t>(- 2.3)</t>
+  </si>
+  <si>
+    <t>(-11.8)</t>
+  </si>
+  <si>
+    <t>(+14.1)</t>
+  </si>
+  <si>
+    <t>(-16.4)</t>
+  </si>
+  <si>
+    <t>(- 4.0)</t>
   </si>
   <si>
     <t>(- 9.1)</t>
   </si>
   <si>
-    <t>(+10.4)</t>
-  </si>
-  <si>
-    <t>(-11.7)</t>
-  </si>
-  <si>
-    <t>Deutschland</t>
+    <t>(+13.1)</t>
+  </si>
+  <si>
+    <t>(-17.1)</t>
+  </si>
+  <si>
+    <t>(- 5.9)</t>
+  </si>
+  <si>
+    <t>(+ 5.3)</t>
+  </si>
+  <si>
+    <t>(- 4.7)</t>
+  </si>
+  <si>
+    <t>(- 6.5)</t>
+  </si>
+  <si>
+    <t>(+ 1.0)</t>
+  </si>
+  <si>
+    <t>(+ 4.5)</t>
+  </si>
+  <si>
+    <t>Kurzfristige Zinsen</t>
+  </si>
+  <si>
+    <t>(- 2.7)</t>
+  </si>
+  <si>
+    <t>(+ 2.8)</t>
+  </si>
+  <si>
+    <t>(- 0.1)</t>
+  </si>
+  <si>
+    <t>(- 2.6)</t>
+  </si>
+  <si>
+    <t>(- 5.3)</t>
+  </si>
+  <si>
+    <t>(+ 3.3)</t>
+  </si>
+  <si>
+    <t>(+ 2.0)</t>
+  </si>
+  <si>
+    <t>(- 1.0)</t>
+  </si>
+  <si>
+    <t>(+ 9.6)</t>
+  </si>
+  <si>
+    <t>(- 8.6)</t>
+  </si>
+  <si>
+    <t>(+ 7.6)</t>
+  </si>
+  <si>
+    <t>Langfristige Zinsen</t>
+  </si>
+  <si>
+    <t>(- 9.0)</t>
+  </si>
+  <si>
+    <t>(+ 5.6)</t>
+  </si>
+  <si>
+    <t>(+ 3.4)</t>
+  </si>
+  <si>
+    <t>(-12.4)</t>
+  </si>
+  <si>
+    <t>(-13.5)</t>
+  </si>
+  <si>
+    <t>(+ 6.0)</t>
+  </si>
+  <si>
+    <t>(+ 7.5)</t>
+  </si>
+  <si>
+    <t>(-21.0)</t>
+  </si>
+  <si>
+    <t>(- 3.3)</t>
+  </si>
+  <si>
+    <t>(+ 2.4)</t>
+  </si>
+  <si>
+    <t>(- 4.2)</t>
+  </si>
+  <si>
+    <t>Aktienkurse</t>
+  </si>
+  <si>
+    <t>STOXX 50 (Euroraum)</t>
+  </si>
+  <si>
+    <t>(+ 6.3)</t>
+  </si>
+  <si>
+    <t>(+ 0.2)</t>
+  </si>
+  <si>
+    <t>(+12.8)</t>
+  </si>
+  <si>
+    <t>DAX (Deutschland)</t>
+  </si>
+  <si>
+    <t>(+ 8.3)</t>
   </si>
   <si>
     <t>(- 2.5)</t>
   </si>
   <si>
-    <t>(- 6.7)</t>
-  </si>
-  <si>
-    <t>(+ 9.2)</t>
-  </si>
-  <si>
-    <t>USA</t>
+    <t>(- 5.8)</t>
+  </si>
+  <si>
+    <t>Dow Jones Industrial (USA)</t>
+  </si>
+  <si>
+    <t>(+ 9.3)</t>
   </si>
   <si>
     <t>(- 4.4)</t>
   </si>
   <si>
-    <t>(- 5.8)</t>
+    <t>(- 4.9)</t>
+  </si>
+  <si>
+    <t>(+14.2)</t>
+  </si>
+  <si>
+    <t>SSE Composite (China)</t>
+  </si>
+  <si>
+    <t>(+ 7.1)</t>
+  </si>
+  <si>
+    <t>(+ 0.5)</t>
+  </si>
+  <si>
+    <t>(- 7.6)</t>
+  </si>
+  <si>
+    <t>(+14.7)</t>
+  </si>
+  <si>
+    <t>Wechselkurse zum Euro</t>
+  </si>
+  <si>
+    <t>aufwerten</t>
+  </si>
+  <si>
+    <t>abwerten</t>
+  </si>
+  <si>
+    <t>Dollar</t>
+  </si>
+  <si>
+    <t>(-13.1)</t>
+  </si>
+  <si>
+    <t>(- 1.9)</t>
+  </si>
+  <si>
+    <t>(+15.0)</t>
+  </si>
+  <si>
+    <t>(-28.1)</t>
+  </si>
+  <si>
+    <t>Yuan</t>
+  </si>
+  <si>
+    <t>(- 5.1)</t>
+  </si>
+  <si>
+    <t>(- 3.4)</t>
+  </si>
+  <si>
+    <t>(+ 8.5)</t>
+  </si>
+  <si>
+    <t>(-13.6)</t>
+  </si>
+  <si>
+    <t>Branchen</t>
+  </si>
+  <si>
+    <t>Banken</t>
+  </si>
+  <si>
+    <t>(+13.4)</t>
+  </si>
+  <si>
+    <t>(- 3.9)</t>
+  </si>
+  <si>
+    <t>(- 9.5)</t>
+  </si>
+  <si>
+    <t>(+22.9)</t>
+  </si>
+  <si>
+    <t>Versicherungen</t>
+  </si>
+  <si>
+    <t>(+16.2)</t>
+  </si>
+  <si>
+    <t>(- 8.7)</t>
+  </si>
+  <si>
+    <t>(- 7.5)</t>
+  </si>
+  <si>
+    <t>(+23.7)</t>
+  </si>
+  <si>
+    <t>Fahrzeuge</t>
+  </si>
+  <si>
+    <t>(+ 3.1)</t>
+  </si>
+  <si>
+    <t>(- 7.1)</t>
+  </si>
+  <si>
+    <t>(+11.1)</t>
+  </si>
+  <si>
+    <t>Chemie/Pharma</t>
+  </si>
+  <si>
+    <t>(+ 8.7)</t>
+  </si>
+  <si>
+    <t>(-15.6)</t>
+  </si>
+  <si>
+    <t>(+24.3)</t>
+  </si>
+  <si>
+    <t>Stahl/NE-Metalle</t>
+  </si>
+  <si>
+    <t>(+ 3.5)</t>
+  </si>
+  <si>
+    <t>(- 7.2)</t>
+  </si>
+  <si>
+    <t>(+10.7)</t>
+  </si>
+  <si>
+    <t>Elektro</t>
+  </si>
+  <si>
+    <t>(+ 8.8)</t>
+  </si>
+  <si>
+    <t>(- 0.8)</t>
+  </si>
+  <si>
+    <t>(- 8.0)</t>
+  </si>
+  <si>
+    <t>(+16.8)</t>
+  </si>
+  <si>
+    <t>Maschinen</t>
+  </si>
+  <si>
+    <t>(+ 6.7)</t>
+  </si>
+  <si>
+    <t>Konsum/Handel</t>
+  </si>
+  <si>
+    <t>(+ 1.7)</t>
+  </si>
+  <si>
+    <t>(+10.3)</t>
+  </si>
+  <si>
+    <t>(-12.0)</t>
+  </si>
+  <si>
+    <t>(+13.7)</t>
+  </si>
+  <si>
+    <t>Bau</t>
+  </si>
+  <si>
+    <t>(+ 1.8)</t>
+  </si>
+  <si>
+    <t>(- 3.6)</t>
+  </si>
+  <si>
+    <t>(+/- 0.0)</t>
+  </si>
+  <si>
+    <t>Versorger</t>
+  </si>
+  <si>
+    <t>(+ 3.9)</t>
+  </si>
+  <si>
+    <t>(- 2.9)</t>
+  </si>
+  <si>
+    <t>(+ 4.9)</t>
+  </si>
+  <si>
+    <t>Dienstleister</t>
+  </si>
+  <si>
+    <t>(+11.6)</t>
+  </si>
+  <si>
+    <t>(-11.5)</t>
+  </si>
+  <si>
+    <t>(+11.4)</t>
+  </si>
+  <si>
+    <t>Telekommunikation</t>
   </si>
   <si>
     <t>(+10.2)</t>
   </si>
   <si>
-    <t>(-14.6)</t>
-  </si>
-  <si>
-    <t>China</t>
-  </si>
-  <si>
-    <t>(+/- 0.0)</t>
-  </si>
-  <si>
-    <t>(- 1.0)</t>
-  </si>
-  <si>
-    <t>(+ 1.0)</t>
-  </si>
-  <si>
-    <t>Konjunktur (Erwartungen)</t>
-  </si>
-  <si>
-    <t>verbessern</t>
-  </si>
-  <si>
-    <t>nicht verändern</t>
-  </si>
-  <si>
-    <t>verschlechtern</t>
-  </si>
-  <si>
-    <t>(+ 2.7)</t>
-  </si>
-  <si>
-    <t>(+ 1.7)</t>
-  </si>
-  <si>
-    <t>(+ 2.6)</t>
-  </si>
-  <si>
-    <t>(- 0.1)</t>
-  </si>
-  <si>
-    <t>(- 1.6)</t>
+    <t>Inform.-Technologien</t>
+  </si>
+  <si>
+    <t>(+ 7.4)</t>
   </si>
   <si>
     <t>(- 2.8)</t>
   </si>
   <si>
-    <t>(+ 4.4)</t>
-  </si>
-  <si>
-    <t>(- 6.0)</t>
-  </si>
-  <si>
-    <t>(+ 3.7)</t>
-  </si>
-  <si>
-    <t>(- 2.1)</t>
-  </si>
-  <si>
-    <t>(+ 0.5)</t>
-  </si>
-  <si>
-    <t>Inflationsrate</t>
-  </si>
-  <si>
-    <t>erhöhen</t>
-  </si>
-  <si>
-    <t>reduzieren</t>
-  </si>
-  <si>
-    <t>(-13.6)</t>
-  </si>
-  <si>
-    <t>(+ 3.5)</t>
-  </si>
-  <si>
-    <t>(+10.1)</t>
-  </si>
-  <si>
-    <t>(-23.7)</t>
-  </si>
-  <si>
-    <t>(-14.2)</t>
-  </si>
-  <si>
-    <t>(+ 2.9)</t>
-  </si>
-  <si>
-    <t>(+11.3)</t>
-  </si>
-  <si>
-    <t>(-25.5)</t>
-  </si>
-  <si>
-    <t>(- 8.8)</t>
-  </si>
-  <si>
-    <t>(- 3.4)</t>
-  </si>
-  <si>
-    <t>(+12.2)</t>
-  </si>
-  <si>
-    <t>(-21.0)</t>
-  </si>
-  <si>
-    <t>(-12.6)</t>
-  </si>
-  <si>
-    <t>(+ 0.4)</t>
-  </si>
-  <si>
-    <t>(-13.0)</t>
-  </si>
-  <si>
-    <t>Kurzfristige Zinsen</t>
-  </si>
-  <si>
-    <t>(- 0.2)</t>
-  </si>
-  <si>
-    <t>(- 0.3)</t>
-  </si>
-  <si>
-    <t>(- 0.7)</t>
-  </si>
-  <si>
-    <t>(- 1.9)</t>
-  </si>
-  <si>
-    <t>(+ 1.4)</t>
-  </si>
-  <si>
-    <t>(- 2.4)</t>
-  </si>
-  <si>
-    <t>(+ 0.8)</t>
-  </si>
-  <si>
-    <t>(+ 1.2)</t>
-  </si>
-  <si>
-    <t>(- 2.0)</t>
-  </si>
-  <si>
-    <t>(+ 2.8)</t>
-  </si>
-  <si>
-    <t>Langfristige Zinsen</t>
-  </si>
-  <si>
-    <t>(- 3.3)</t>
-  </si>
-  <si>
-    <t>(+ 0.1)</t>
-  </si>
-  <si>
-    <t>(+ 3.2)</t>
-  </si>
-  <si>
-    <t>(- 6.5)</t>
-  </si>
-  <si>
-    <t>(- 3.9)</t>
-  </si>
-  <si>
-    <t>(- 2.3)</t>
-  </si>
-  <si>
-    <t>(+ 6.2)</t>
-  </si>
-  <si>
-    <t>(-10.1)</t>
-  </si>
-  <si>
-    <t>(- 0.8)</t>
-  </si>
-  <si>
-    <t>(- 1.2)</t>
-  </si>
-  <si>
-    <t>Aktienkurse</t>
-  </si>
-  <si>
-    <t>STOXX 50 (Euroraum)</t>
-  </si>
-  <si>
-    <t>(+ 1.9)</t>
-  </si>
-  <si>
-    <t>(- 4.8)</t>
-  </si>
-  <si>
-    <t>(+ 7.7)</t>
-  </si>
-  <si>
-    <t>DAX (Deutschland)</t>
-  </si>
-  <si>
-    <t>(+ 3.1)</t>
-  </si>
-  <si>
-    <t>(+ 0.9)</t>
-  </si>
-  <si>
-    <t>(- 4.0)</t>
-  </si>
-  <si>
-    <t>(+ 7.1)</t>
-  </si>
-  <si>
-    <t>Dow Jones Industrial (USA)</t>
-  </si>
-  <si>
-    <t>(- 0.4)</t>
-  </si>
-  <si>
-    <t>SSE Composite (China)</t>
-  </si>
-  <si>
-    <t>(- 3.0)</t>
-  </si>
-  <si>
-    <t>(+ 3.8)</t>
-  </si>
-  <si>
-    <t>(- 6.8)</t>
-  </si>
-  <si>
-    <t>Wechselkurse zum Euro</t>
-  </si>
-  <si>
-    <t>aufwerten</t>
-  </si>
-  <si>
-    <t>abwerten</t>
-  </si>
-  <si>
-    <t>Dollar</t>
-  </si>
-  <si>
-    <t>(- 3.1)</t>
-  </si>
-  <si>
-    <t>(- 4.1)</t>
-  </si>
-  <si>
-    <t>(+ 7.2)</t>
-  </si>
-  <si>
-    <t>(-10.3)</t>
-  </si>
-  <si>
-    <t>Yuan</t>
-  </si>
-  <si>
-    <t>(+ 0.7)</t>
-  </si>
-  <si>
-    <t>Branchen</t>
-  </si>
-  <si>
-    <t>Banken</t>
-  </si>
-  <si>
-    <t>(+ 5.4)</t>
-  </si>
-  <si>
-    <t>(- 8.4)</t>
-  </si>
-  <si>
-    <t>Versicherungen</t>
-  </si>
-  <si>
-    <t>(- 6.4)</t>
-  </si>
-  <si>
-    <t>(+ 1.5)</t>
-  </si>
-  <si>
-    <t>(+ 4.9)</t>
-  </si>
-  <si>
-    <t>(-11.3)</t>
-  </si>
-  <si>
-    <t>Fahrzeuge</t>
-  </si>
-  <si>
-    <t>(- 2.6)</t>
-  </si>
-  <si>
-    <t>Chemie/Pharma</t>
-  </si>
-  <si>
-    <t>(- 5.0)</t>
-  </si>
-  <si>
-    <t>(- 2.2)</t>
-  </si>
-  <si>
-    <t>Stahl/NE-Metalle</t>
-  </si>
-  <si>
-    <t>(+ 3.9)</t>
-  </si>
-  <si>
-    <t>(- 6.2)</t>
-  </si>
-  <si>
-    <t>Elektro</t>
-  </si>
-  <si>
-    <t>(+ 1.3)</t>
-  </si>
-  <si>
-    <t>(- 3.8)</t>
-  </si>
-  <si>
-    <t>Maschinen</t>
-  </si>
-  <si>
-    <t>(- 0.5)</t>
-  </si>
-  <si>
-    <t>Konsum/Handel</t>
-  </si>
-  <si>
-    <t>(- 2.7)</t>
-  </si>
-  <si>
-    <t>(- 4.7)</t>
-  </si>
-  <si>
-    <t>Bau</t>
-  </si>
-  <si>
-    <t>(- 3.5)</t>
-  </si>
-  <si>
-    <t>(+ 5.7)</t>
-  </si>
-  <si>
-    <t>(- 7.9)</t>
-  </si>
-  <si>
-    <t>Versorger</t>
-  </si>
-  <si>
-    <t>(+12.7)</t>
-  </si>
-  <si>
-    <t>(- 5.9)</t>
-  </si>
-  <si>
-    <t>(- 0.9)</t>
-  </si>
-  <si>
-    <t>Dienstleister</t>
-  </si>
-  <si>
-    <t>(-11.0)</t>
-  </si>
-  <si>
-    <t>Telekommunikation</t>
-  </si>
-  <si>
-    <t>(- 7.1)</t>
-  </si>
-  <si>
-    <t>(+ 6.9)</t>
-  </si>
-  <si>
-    <t>(+ 0.2)</t>
-  </si>
-  <si>
-    <t>(- 7.3)</t>
-  </si>
-  <si>
-    <t>Inform.-Technologien</t>
-  </si>
-  <si>
-    <t>(- 7.6)</t>
-  </si>
-  <si>
-    <t>(+ 5.6)</t>
-  </si>
-  <si>
-    <t>(+ 2.0)</t>
-  </si>
-  <si>
-    <t>(- 9.6)</t>
-  </si>
-  <si>
-    <t>Bemerkung: An der Oktober-Umfrage des Finanzmarkttests vom 10.10.2022 - 17.10.2022 beteiligten sich 176 Analysten. Abgefragt</t>
+    <t>(+12.0)</t>
+  </si>
+  <si>
+    <t>Bemerkung: An der November-Umfrage des Finanzmarkttests vom 7.11.2022 - 14.11.2022 beteiligten sich 193 Analysten. Abgefragt</t>
   </si>
   <si>
     <t>wurden die Erwartungen für die kommenden sechs Monate. Dargestellt sind die prozentualen Anteile der Antwortkategorien, in Klammern</t>
@@ -1325,25 +1388,25 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>1.2</v>
+        <v>2.1</v>
       </c>
       <c r="D5" t="s">
         <v>8</v>
       </c>
       <c r="E5">
-        <v>27</v>
+        <v>30.7</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
       </c>
       <c r="G5">
-        <v>71.8</v>
+        <v>67.2</v>
       </c>
       <c r="H5" t="s">
         <v>10</v>
       </c>
       <c r="I5">
-        <v>-70.599999999999994</v>
+        <v>-65.099999999999994</v>
       </c>
       <c r="J5" t="s">
         <v>11</v>
@@ -1354,100 +1417,100 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>1.2</v>
+        <v>1.6</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
       </c>
       <c r="E6">
-        <v>25.4</v>
+        <v>32.299999999999997</v>
       </c>
       <c r="F6" t="s">
         <v>14</v>
       </c>
       <c r="G6">
-        <v>73.400000000000006</v>
+        <v>66.099999999999994</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
       </c>
       <c r="I6">
-        <v>-72.2</v>
+        <v>-64.5</v>
       </c>
       <c r="J6" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7">
-        <v>15.1</v>
+        <v>13.6</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E7">
-        <v>56.4</v>
+        <v>65.3</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G7">
-        <v>28.5</v>
+        <v>21.1</v>
       </c>
       <c r="H7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="I7">
-        <v>-13.4</v>
+        <v>-7.5</v>
       </c>
       <c r="J7" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C8">
-        <v>0</v>
+        <v>1.2</v>
       </c>
       <c r="D8" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E8">
-        <v>30.8</v>
+        <v>31.4</v>
       </c>
       <c r="F8" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G8">
-        <v>69.2</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="H8" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I8">
-        <v>-69.2</v>
+        <v>-66.2</v>
       </c>
       <c r="J8" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E10" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G10" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I10" t="s">
         <v>6</v>
@@ -1458,28 +1521,28 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>7.5</v>
+        <v>12.6</v>
       </c>
       <c r="D11" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E11">
-        <v>25.3</v>
+        <v>36.1</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="G11">
-        <v>67.2</v>
+        <v>51.3</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="I11">
-        <v>-59.7</v>
+        <v>-38.700000000000003</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="2:10" x14ac:dyDescent="0.3">
@@ -1487,100 +1550,100 @@
         <v>12</v>
       </c>
       <c r="C12">
-        <v>8.6</v>
+        <v>14.1</v>
       </c>
       <c r="D12" t="s">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="E12">
-        <v>23.6</v>
+        <v>35.1</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>35</v>
       </c>
       <c r="G12">
-        <v>67.8</v>
+        <v>50.8</v>
       </c>
       <c r="H12" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="I12">
-        <v>-59.2</v>
+        <v>-36.700000000000003</v>
       </c>
       <c r="J12" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13">
-        <v>7.6</v>
+        <v>11.6</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="E13">
-        <v>39.200000000000003</v>
+        <v>41.3</v>
       </c>
       <c r="F13" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
       <c r="G13">
-        <v>53.2</v>
+        <v>47.1</v>
       </c>
       <c r="H13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="I13">
-        <v>-45.6</v>
+        <v>-35.5</v>
       </c>
       <c r="J13" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C14">
-        <v>15.9</v>
+        <v>24.9</v>
       </c>
       <c r="D14" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="E14">
-        <v>54.4</v>
+        <v>52</v>
       </c>
       <c r="F14" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G14">
-        <v>29.7</v>
+        <v>23.1</v>
       </c>
       <c r="H14" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="I14">
-        <v>-13.8</v>
+        <v>1.8</v>
       </c>
       <c r="J14" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G16" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I16" t="s">
         <v>6</v>
@@ -1591,28 +1654,28 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>13.3</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="E17">
-        <v>37.6</v>
+        <v>25.8</v>
       </c>
       <c r="F17" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="G17">
-        <v>49.1</v>
+        <v>63.2</v>
       </c>
       <c r="H17" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="I17">
-        <v>-35.799999999999997</v>
+        <v>-52.2</v>
       </c>
       <c r="J17" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.3">
@@ -1620,100 +1683,100 @@
         <v>12</v>
       </c>
       <c r="C18">
-        <v>14.5</v>
+        <v>10.5</v>
       </c>
       <c r="D18" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="E18">
-        <v>35.799999999999997</v>
+        <v>26.7</v>
       </c>
       <c r="F18" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G18">
-        <v>49.7</v>
+        <v>62.8</v>
       </c>
       <c r="H18" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="I18">
-        <v>-35.200000000000003</v>
+        <v>-52.3</v>
       </c>
       <c r="J18" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B19" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C19">
-        <v>5.2</v>
+        <v>5.8</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="E19">
-        <v>18.600000000000001</v>
+        <v>12.7</v>
       </c>
       <c r="F19" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="G19">
-        <v>76.2</v>
+        <v>81.5</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="I19">
-        <v>-71</v>
+        <v>-75.7</v>
       </c>
       <c r="J19" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C20">
-        <v>6.5</v>
+        <v>12</v>
       </c>
       <c r="D20" t="s">
-        <v>55</v>
+        <v>11</v>
       </c>
       <c r="E20">
-        <v>72.5</v>
+        <v>66</v>
       </c>
       <c r="F20" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="G20">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="I20">
-        <v>-14.5</v>
+        <v>-10</v>
       </c>
       <c r="J20" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="C22" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E22" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G22" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I22" t="s">
         <v>6</v>
@@ -1724,100 +1787,100 @@
         <v>7</v>
       </c>
       <c r="C23">
-        <v>94.3</v>
+        <v>91.6</v>
       </c>
       <c r="D23" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="E23">
-        <v>4</v>
+        <v>6.8</v>
       </c>
       <c r="F23" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="G23">
-        <v>1.7</v>
+        <v>1.6</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>66</v>
       </c>
       <c r="I23">
-        <v>92.6</v>
+        <v>90</v>
       </c>
       <c r="J23" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C24">
-        <v>89</v>
+        <v>83.7</v>
       </c>
       <c r="D24" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E24">
-        <v>9.3000000000000007</v>
+        <v>12.6</v>
       </c>
       <c r="F24" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="G24">
-        <v>1.7</v>
+        <v>3.7</v>
       </c>
       <c r="H24" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="I24">
-        <v>87.3</v>
+        <v>80</v>
       </c>
       <c r="J24" t="s">
-        <v>64</v>
+        <v>15</v>
       </c>
     </row>
     <row r="25" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C25">
-        <v>24.8</v>
+        <v>23.8</v>
       </c>
       <c r="D25" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E25">
-        <v>58.4</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="G25">
-        <v>16.8</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="H25" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="I25">
-        <v>8</v>
+        <v>15.6</v>
       </c>
       <c r="J25" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B27" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C27" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E27" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G27" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I27" t="s">
         <v>6</v>
@@ -1828,100 +1891,100 @@
         <v>12</v>
       </c>
       <c r="C28">
-        <v>61.1</v>
+        <v>52.1</v>
       </c>
       <c r="D28" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="E28">
-        <v>26.5</v>
+        <v>32.1</v>
       </c>
       <c r="F28" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="G28">
-        <v>12.4</v>
+        <v>15.8</v>
       </c>
       <c r="H28" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="I28">
-        <v>48.7</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="J28" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B29" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C29">
-        <v>55.3</v>
+        <v>41.8</v>
       </c>
       <c r="D29" t="s">
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="E29">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F29" t="s">
-        <v>75</v>
+        <v>81</v>
       </c>
       <c r="G29">
-        <v>14.7</v>
+        <v>22.2</v>
       </c>
       <c r="H29" t="s">
-        <v>76</v>
+        <v>82</v>
       </c>
       <c r="I29">
-        <v>40.6</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="J29" t="s">
-        <v>77</v>
+        <v>83</v>
       </c>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B30" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C30">
-        <v>26.1</v>
+        <v>22.8</v>
       </c>
       <c r="D30" t="s">
-        <v>78</v>
+        <v>84</v>
       </c>
       <c r="E30">
-        <v>63.1</v>
+        <v>65.5</v>
       </c>
       <c r="F30" t="s">
-        <v>56</v>
+        <v>85</v>
       </c>
       <c r="G30">
-        <v>10.8</v>
+        <v>11.7</v>
       </c>
       <c r="H30" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="I30">
-        <v>15.3</v>
+        <v>11.1</v>
       </c>
       <c r="J30" t="s">
-        <v>79</v>
+        <v>86</v>
       </c>
     </row>
     <row r="32" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B32" t="s">
-        <v>80</v>
+        <v>87</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="E32" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G32" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I32" t="s">
         <v>6</v>
@@ -1929,132 +1992,132 @@
     </row>
     <row r="33" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B33" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="C33">
-        <v>32.1</v>
+        <v>38.4</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>89</v>
       </c>
       <c r="E33">
-        <v>38.299999999999997</v>
+        <v>38.5</v>
       </c>
       <c r="F33" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="G33">
-        <v>29.6</v>
+        <v>23.1</v>
       </c>
       <c r="H33" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="I33">
-        <v>2.5</v>
+        <v>15.3</v>
       </c>
       <c r="J33" t="s">
-        <v>84</v>
+        <v>91</v>
       </c>
     </row>
     <row r="34" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B34" t="s">
-        <v>85</v>
+        <v>92</v>
       </c>
       <c r="C34">
-        <v>32.299999999999997</v>
+        <v>40.6</v>
       </c>
       <c r="D34" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="E34">
-        <v>36.6</v>
+        <v>34.1</v>
       </c>
       <c r="F34" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="G34">
-        <v>31.1</v>
+        <v>25.3</v>
       </c>
       <c r="H34" t="s">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="I34">
-        <v>1.2</v>
+        <v>15.3</v>
       </c>
       <c r="J34" t="s">
-        <v>89</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B35" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C35">
-        <v>35.799999999999997</v>
+        <v>45.1</v>
       </c>
       <c r="D35" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="E35">
-        <v>40.1</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="F35" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="G35">
-        <v>24.1</v>
+        <v>19.2</v>
       </c>
       <c r="H35" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="I35">
-        <v>11.7</v>
+        <v>25.9</v>
       </c>
       <c r="J35" t="s">
-        <v>78</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B36" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C36">
-        <v>30.8</v>
+        <v>37.9</v>
       </c>
       <c r="D36" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="E36">
-        <v>44.6</v>
+        <v>45.1</v>
       </c>
       <c r="F36" t="s">
-        <v>78</v>
+        <v>103</v>
       </c>
       <c r="G36">
-        <v>24.6</v>
+        <v>17</v>
       </c>
       <c r="H36" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="I36">
-        <v>6.2</v>
+        <v>20.9</v>
       </c>
       <c r="J36" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
     </row>
     <row r="38" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B38" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="C38" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="E38" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G38" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="I38" t="s">
         <v>6</v>
@@ -2062,74 +2125,74 @@
     </row>
     <row r="39" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B39" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="C39">
-        <v>33</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="D39" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="E39">
-        <v>38.9</v>
+        <v>37</v>
       </c>
       <c r="F39" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="G39">
-        <v>28.1</v>
+        <v>43.1</v>
       </c>
       <c r="H39" t="s">
-        <v>102</v>
+        <v>112</v>
       </c>
       <c r="I39">
-        <v>4.9000000000000004</v>
+        <v>-23.2</v>
       </c>
       <c r="J39" t="s">
-        <v>103</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B40" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="C40">
-        <v>20.399999999999999</v>
+        <v>15.3</v>
       </c>
       <c r="D40" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E40">
-        <v>56.2</v>
+        <v>52.8</v>
       </c>
       <c r="F40" t="s">
-        <v>38</v>
+        <v>116</v>
       </c>
       <c r="G40">
-        <v>23.4</v>
+        <v>31.9</v>
       </c>
       <c r="H40" t="s">
-        <v>63</v>
+        <v>117</v>
       </c>
       <c r="I40">
-        <v>-3</v>
+        <v>-16.600000000000001</v>
       </c>
       <c r="J40" t="s">
-        <v>61</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B42" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="C42" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E42" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G42" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I42" t="s">
         <v>6</v>
@@ -2137,394 +2200,394 @@
     </row>
     <row r="43" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
-        <v>107</v>
+        <v>120</v>
       </c>
       <c r="C43">
-        <v>37.5</v>
+        <v>50.9</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>121</v>
       </c>
       <c r="E43">
-        <v>30.9</v>
+        <v>27</v>
       </c>
       <c r="F43" t="s">
-        <v>64</v>
+        <v>122</v>
       </c>
       <c r="G43">
-        <v>31.6</v>
+        <v>22.1</v>
       </c>
       <c r="H43" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="I43">
-        <v>5.9</v>
+        <v>28.8</v>
       </c>
       <c r="J43" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B44" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="C44">
-        <v>29.1</v>
+        <v>45.3</v>
       </c>
       <c r="D44" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E44">
-        <v>49.7</v>
+        <v>41</v>
       </c>
       <c r="F44" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="G44">
-        <v>21.2</v>
+        <v>13.7</v>
       </c>
       <c r="H44" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="I44">
-        <v>7.9</v>
+        <v>31.6</v>
       </c>
       <c r="J44" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
     </row>
     <row r="45" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B45" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="C45">
-        <v>4.5999999999999996</v>
+        <v>8.6</v>
       </c>
       <c r="D45" t="s">
-        <v>116</v>
+        <v>38</v>
       </c>
       <c r="E45">
-        <v>27.6</v>
+        <v>30.7</v>
       </c>
       <c r="F45" t="s">
-        <v>66</v>
+        <v>131</v>
       </c>
       <c r="G45">
-        <v>67.8</v>
+        <v>60.7</v>
       </c>
       <c r="H45" t="s">
-        <v>63</v>
+        <v>132</v>
       </c>
       <c r="I45">
-        <v>-63.2</v>
+        <v>-52.1</v>
       </c>
       <c r="J45" t="s">
-        <v>88</v>
+        <v>133</v>
       </c>
     </row>
     <row r="46" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B46" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="C46">
-        <v>8</v>
+        <v>16.7</v>
       </c>
       <c r="D46" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="E46">
-        <v>27.3</v>
+        <v>34.200000000000003</v>
       </c>
       <c r="F46" t="s">
-        <v>102</v>
+        <v>14</v>
       </c>
       <c r="G46">
-        <v>64.7</v>
+        <v>49.1</v>
       </c>
       <c r="H46" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="I46">
-        <v>-56.7</v>
+        <v>-32.4</v>
       </c>
       <c r="J46" t="s">
-        <v>34</v>
+        <v>137</v>
       </c>
     </row>
     <row r="47" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B47" t="s">
-        <v>120</v>
+        <v>138</v>
       </c>
       <c r="C47">
-        <v>2.7</v>
+        <v>6.2</v>
       </c>
       <c r="D47" t="s">
-        <v>75</v>
+        <v>139</v>
       </c>
       <c r="E47">
-        <v>19.3</v>
+        <v>23</v>
       </c>
       <c r="F47" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="G47">
-        <v>78</v>
+        <v>70.8</v>
       </c>
       <c r="H47" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="I47">
-        <v>-75.3</v>
+        <v>-64.599999999999994</v>
       </c>
       <c r="J47" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
     </row>
     <row r="48" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B48" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="C48">
-        <v>6.1</v>
+        <v>14.9</v>
       </c>
       <c r="D48" t="s">
-        <v>13</v>
+        <v>143</v>
       </c>
       <c r="E48">
-        <v>53</v>
+        <v>52.2</v>
       </c>
       <c r="F48" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="G48">
-        <v>40.9</v>
+        <v>32.9</v>
       </c>
       <c r="H48" t="s">
-        <v>124</v>
+        <v>145</v>
       </c>
       <c r="I48">
-        <v>-34.799999999999997</v>
+        <v>-18</v>
       </c>
       <c r="J48" t="s">
-        <v>125</v>
+        <v>146</v>
       </c>
     </row>
     <row r="49" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B49" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="C49">
-        <v>4.8</v>
+        <v>6.8</v>
       </c>
       <c r="D49" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="E49">
-        <v>29.7</v>
+        <v>36.4</v>
       </c>
       <c r="F49" t="s">
+        <v>148</v>
+      </c>
+      <c r="G49">
+        <v>56.8</v>
+      </c>
+      <c r="H49" t="s">
         <v>127</v>
       </c>
-      <c r="G49">
-        <v>65.5</v>
-      </c>
-      <c r="H49" t="s">
-        <v>22</v>
-      </c>
       <c r="I49">
-        <v>-60.7</v>
+        <v>-50</v>
       </c>
       <c r="J49" t="s">
-        <v>39</v>
+        <v>141</v>
       </c>
     </row>
     <row r="50" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B50" t="s">
-        <v>128</v>
+        <v>149</v>
       </c>
       <c r="C50">
-        <v>3.3</v>
+        <v>5</v>
       </c>
       <c r="D50" t="s">
-        <v>23</v>
+        <v>150</v>
       </c>
       <c r="E50">
-        <v>18.7</v>
+        <v>29</v>
       </c>
       <c r="F50" t="s">
-        <v>129</v>
+        <v>151</v>
       </c>
       <c r="G50">
-        <v>78</v>
+        <v>66</v>
       </c>
       <c r="H50" t="s">
-        <v>37</v>
+        <v>152</v>
       </c>
       <c r="I50">
-        <v>-74.7</v>
+        <v>-61</v>
       </c>
       <c r="J50" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
     </row>
     <row r="51" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B51" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="C51">
-        <v>0</v>
+        <v>1.8</v>
       </c>
       <c r="D51" t="s">
-        <v>119</v>
+        <v>155</v>
       </c>
       <c r="E51">
-        <v>17.2</v>
+        <v>13.6</v>
       </c>
       <c r="F51" t="s">
-        <v>132</v>
+        <v>156</v>
       </c>
       <c r="G51">
-        <v>82.8</v>
+        <v>84.6</v>
       </c>
       <c r="H51" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
       <c r="I51">
         <v>-82.8</v>
       </c>
       <c r="J51" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
     </row>
     <row r="52" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B52" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="C52">
-        <v>25.3</v>
+        <v>29.2</v>
       </c>
       <c r="D52" t="s">
-        <v>95</v>
+        <v>159</v>
       </c>
       <c r="E52">
-        <v>52</v>
+        <v>49.1</v>
       </c>
       <c r="F52" t="s">
-        <v>136</v>
+        <v>160</v>
       </c>
       <c r="G52">
-        <v>22.7</v>
+        <v>21.7</v>
       </c>
       <c r="H52" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
       <c r="I52">
-        <v>2.6</v>
+        <v>7.5</v>
       </c>
       <c r="J52" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
     </row>
     <row r="53" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B53" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="C53">
-        <v>10.6</v>
+        <v>10.5</v>
       </c>
       <c r="D53" t="s">
-        <v>125</v>
+        <v>66</v>
       </c>
       <c r="E53">
-        <v>56.3</v>
+        <v>67.900000000000006</v>
       </c>
       <c r="F53" t="s">
-        <v>52</v>
+        <v>163</v>
       </c>
       <c r="G53">
-        <v>33.1</v>
+        <v>21.6</v>
       </c>
       <c r="H53" t="s">
-        <v>102</v>
+        <v>164</v>
       </c>
       <c r="I53">
-        <v>-22.5</v>
+        <v>-11.1</v>
       </c>
       <c r="J53" t="s">
-        <v>140</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B54" t="s">
-        <v>141</v>
+        <v>166</v>
       </c>
       <c r="C54">
-        <v>15</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="D54" t="s">
-        <v>142</v>
+        <v>31</v>
       </c>
       <c r="E54">
         <v>75.5</v>
       </c>
       <c r="F54" t="s">
-        <v>143</v>
+        <v>157</v>
       </c>
       <c r="G54">
-        <v>9.5</v>
+        <v>4.4000000000000004</v>
       </c>
       <c r="H54" t="s">
-        <v>144</v>
+        <v>115</v>
       </c>
       <c r="I54">
-        <v>5.5</v>
+        <v>15.7</v>
       </c>
       <c r="J54" t="s">
-        <v>145</v>
+        <v>167</v>
       </c>
     </row>
     <row r="55" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B55" t="s">
-        <v>146</v>
+        <v>168</v>
       </c>
       <c r="C55">
-        <v>26.2</v>
+        <v>33.6</v>
       </c>
       <c r="D55" t="s">
-        <v>147</v>
+        <v>169</v>
       </c>
       <c r="E55">
-        <v>62.4</v>
+        <v>59.6</v>
       </c>
       <c r="F55" t="s">
-        <v>148</v>
+        <v>170</v>
       </c>
       <c r="G55">
-        <v>11.4</v>
+        <v>6.8</v>
       </c>
       <c r="H55" t="s">
-        <v>149</v>
+        <v>10</v>
       </c>
       <c r="I55">
-        <v>14.8</v>
+        <v>26.8</v>
       </c>
       <c r="J55" t="s">
-        <v>150</v>
+        <v>171</v>
       </c>
     </row>
     <row r="57" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B57" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
     </row>
     <row r="58" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B58" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="2:10" x14ac:dyDescent="0.3">
       <c r="B59" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
     </row>
   </sheetData>

</xml_diff>